<commit_message>
se realizan nuevos cambios version estable
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos.xlsx
@@ -8,6 +8,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$K$2</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
@@ -109,10 +112,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -133,16 +136,16 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -150,14 +153,11 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,19 +708,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="100" workbookViewId="0">
       <selection activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="4"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="2" width="22.8515625"/>
-    <col customWidth="1" min="3" max="3" style="2" width="24.7109375"/>
-    <col customWidth="1" min="4" max="4" style="2" width="17.28125"/>
-    <col customWidth="1" min="5" max="8" width="17.28125"/>
-    <col customWidth="1" min="9" max="9" width="34.57421875"/>
-    <col customWidth="1" min="10" max="11" width="17.28125"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="4"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="22.8515625"/>
+    <col customWidth="1" min="3" max="3" style="1" width="24.7109375"/>
+    <col customWidth="1" min="4" max="8" style="1" width="17.28125"/>
+    <col customWidth="1" min="9" max="9" style="1" width="34.57421875"/>
+    <col customWidth="1" min="10" max="11" style="1" width="17.28125"/>
+    <col min="12" max="16384" style="1" width="11.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="43.5" customHeight="1">
@@ -738,72 +738,73 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" s="6" customFormat="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" s="1" customFormat="1">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="D13" s="2"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="D14" s="2"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="D15" s="2"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="D16" s="2"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="D17" s="2"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="D18" s="2"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="D19" s="2"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="D20" s="2"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="D21" s="2"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="D22" s="2"/>
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="B2:K2"/>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:K1"/>

</xml_diff>

<commit_message>
se hacen ajustes en las vistas
</commit_message>
<xml_diff>
--- a/src/Views/assets/excel/reporte-almuerzos.xlsx
+++ b/src/Views/assets/excel/reporte-almuerzos.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$2:$L$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$K$2</definedName>
   </definedNames>
   <calcPr/>
@@ -24,6 +25,9 @@
     <t>#</t>
   </si>
   <si>
+    <t>Fecha</t>
+  </si>
+  <si>
     <t xml:space="preserve">Numero de Identificacion</t>
   </si>
   <si>
@@ -49,9 +53,6 @@
   </si>
   <si>
     <t>Bebida</t>
-  </si>
-  <si>
-    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -113,7 +114,9 @@
         <color auto="1"/>
       </left>
       <right style="none"/>
-      <top style="none"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
@@ -136,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -147,16 +150,22 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -178,15 +187,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
+      <xdr:colOff>123823</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>990599</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>552449</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -201,9 +210,9 @@
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="123825" y="1"/>
-          <a:ext cx="1333500" cy="552450"/>
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="123823" y="0"/>
+          <a:ext cx="2247900" cy="552449"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,28 +717,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="4"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="22.8515625"/>
-    <col customWidth="1" min="3" max="3" style="1" width="24.7109375"/>
-    <col customWidth="1" min="4" max="8" style="1" width="17.28125"/>
-    <col customWidth="1" min="9" max="9" style="1" width="34.57421875"/>
-    <col customWidth="1" min="10" max="11" style="1" width="17.28125"/>
-    <col min="12" max="16384" style="1" width="11.421875"/>
+    <col customWidth="1" min="2" max="2" style="2" width="16.7109375"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="22.8515625"/>
+    <col customWidth="1" min="4" max="4" style="1" width="24.7109375"/>
+    <col customWidth="1" min="5" max="9" style="1" width="17.28125"/>
+    <col customWidth="1" min="10" max="10" style="1" width="34.57421875"/>
+    <col customWidth="1" min="11" max="12" style="1" width="17.28125"/>
+    <col min="13" max="16384" style="1" width="11.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="43.5" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -737,77 +747,79 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" s="1" customFormat="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="9"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" ht="14.25">
-      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:K2"/>
   <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:K1"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>